<commit_message>
Add unique VINs to Each CA Select Test PT1
</commit_message>
<xml_diff>
--- a/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_CA_SELECT.xlsx
+++ b/aaa-automation-tests/src/test/resources/uploadingfiles/vinUploadFiles/NewVIN_CA_SELECT.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT-repo\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gp8john\Documents\CSAA\pas-cvqaautomation\aaa-automation-tests\src\test\resources\uploadingfiles\vinUploadFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9732"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>TEST</t>
   </si>
   <si>
-    <t>1FDEU15H&amp;K</t>
-  </si>
-  <si>
     <t>STAT</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>BODYSTYLEPAS2713ENDOR</t>
+  </si>
+  <si>
+    <t>AAANK3CC&amp;F</t>
   </si>
 </sst>
 </file>
@@ -659,34 +659,34 @@
   <dimension ref="A1:AL7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="6" max="6" width="14.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="10" max="10" width="14.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.77734375" customWidth="1"/>
-    <col min="19" max="19" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.88671875" customWidth="1"/>
-    <col min="23" max="23" width="22.21875" customWidth="1"/>
-    <col min="24" max="24" width="20.88671875" customWidth="1"/>
-    <col min="25" max="25" width="34.77734375" customWidth="1"/>
-    <col min="26" max="26" width="8.21875" customWidth="1"/>
-    <col min="27" max="27" width="14.88671875" customWidth="1"/>
-    <col min="28" max="29" width="16.21875" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.7109375" customWidth="1"/>
+    <col min="19" max="19" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.85546875" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.85546875" customWidth="1"/>
+    <col min="25" max="25" width="34.7109375" customWidth="1"/>
+    <col min="26" max="26" width="8.28515625" customWidth="1"/>
+    <col min="27" max="27" width="14.85546875" customWidth="1"/>
+    <col min="28" max="29" width="16.28515625" customWidth="1"/>
     <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="21.44140625" customWidth="1"/>
+    <col min="38" max="38" width="21.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -763,7 +763,7 @@
         <v>24</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AA1" s="1" t="s">
         <v>25</v>
@@ -772,7 +772,7 @@
         <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AD1" s="1" t="s">
         <v>27</v>
@@ -802,21 +802,21 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="2">
         <v>2018</v>
       </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
         <v>40</v>
@@ -892,16 +892,16 @@
         <v>39</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AI2">
         <v>20010101</v>
@@ -916,24 +916,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="2">
         <v>2018</v>
       </c>
       <c r="D3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
         <v>56</v>
       </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
       <c r="F3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>28</v>
@@ -1006,16 +1006,16 @@
         <v>39</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AH3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AI3">
         <v>20000101</v>
@@ -1030,24 +1030,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="2">
         <v>2018</v>
       </c>
       <c r="D4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E4" t="s">
         <v>56</v>
       </c>
-      <c r="E4" t="s">
-        <v>57</v>
-      </c>
       <c r="F4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>28</v>
@@ -1120,16 +1120,16 @@
         <v>39</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI4">
         <v>20150101</v>
@@ -1144,24 +1144,24 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5" s="2">
         <v>2018</v>
       </c>
       <c r="D5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s">
         <v>56</v>
       </c>
-      <c r="E5" t="s">
-        <v>57</v>
-      </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>28</v>
@@ -1221,7 +1221,7 @@
         <v>37</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AA5" s="2">
         <v>41</v>
@@ -1234,16 +1234,16 @@
         <v>39</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AH5" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AI5">
         <v>20190101</v>
@@ -1258,27 +1258,27 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C6" s="2">
         <v>2018</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="H6" s="3">
         <v>88888</v>
@@ -1287,19 +1287,19 @@
         <v>29</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O6" s="3">
         <v>12</v>
@@ -1311,7 +1311,7 @@
         <v>214</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S6" s="3">
         <v>4</v>
@@ -1335,7 +1335,7 @@
         <v>37</v>
       </c>
       <c r="Z6" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA6" s="3">
         <v>33</v>
@@ -1347,16 +1347,16 @@
         <v>39</v>
       </c>
       <c r="AE6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI6" s="3">
         <v>20000101</v>
@@ -1371,27 +1371,27 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>2018</v>
       </c>
       <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
         <v>76</v>
       </c>
-      <c r="E7" t="s">
-        <v>76</v>
-      </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>77</v>
-      </c>
-      <c r="G7" t="s">
-        <v>78</v>
       </c>
       <c r="H7">
         <v>88888</v>
@@ -1400,19 +1400,19 @@
         <v>29</v>
       </c>
       <c r="J7" t="s">
+        <v>78</v>
+      </c>
+      <c r="K7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" t="s">
         <v>79</v>
-      </c>
-      <c r="K7" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" t="s">
-        <v>80</v>
       </c>
       <c r="M7" t="s">
         <v>29</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O7">
         <v>12</v>
@@ -1424,7 +1424,7 @@
         <v>214</v>
       </c>
       <c r="R7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S7">
         <v>4</v>
@@ -1448,7 +1448,7 @@
         <v>37</v>
       </c>
       <c r="Z7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AA7">
         <v>33</v>
@@ -1457,22 +1457,22 @@
         <v>43</v>
       </c>
       <c r="AC7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AD7" t="s">
         <v>39</v>
       </c>
       <c r="AE7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI7">
         <v>20000101</v>

</xml_diff>